<commit_message>
Updated tast description document
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Task001</t>
   </si>
   <si>
-    <t>Commit file to Repo</t>
-  </si>
-  <si>
     <t>Task002</t>
   </si>
   <si>
@@ -54,15 +51,78 @@
     <t>Task010</t>
   </si>
   <si>
-    <t>Restore file from Repo</t>
+    <t>Restore file from Repo using hash and given name</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create commit command with syntax "commit </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>filename</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" that saves file to repo</t>
+    </r>
+  </si>
+  <si>
+    <t>Save file to repo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create restore command with syntax "restore </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hash filename</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" that restores file from hash and gives it the given name</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -375,12 +435,12 @@
   <dimension ref="A2:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="69.85546875" customWidth="1"/>
+    <col min="3" max="3" width="147.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -391,7 +451,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -399,10 +459,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -410,7 +470,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -418,7 +481,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -426,7 +492,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -434,7 +500,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -442,7 +508,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -450,7 +516,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -458,7 +524,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -466,10 +532,11 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>